<commit_message>
add count of leads
</commit_message>
<xml_diff>
--- a/data/leads.xlsx
+++ b/data/leads.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="132">
   <si>
     <t>Company</t>
   </si>
@@ -412,6 +412,9 @@
   </si>
   <si>
     <t>Enjoys long walks along the beach in Mexico</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -777,7 +780,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,7 +791,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>42</v>
+        <v>131</v>
       </c>
       <c r="B1">
         <v>1</v>

</xml_diff>

<commit_message>
add leadscore to dataset
</commit_message>
<xml_diff>
--- a/data/leads.xlsx
+++ b/data/leads.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="131">
   <si>
     <t>Company</t>
   </si>
@@ -147,9 +147,6 @@
     <t>Details-Product2</t>
   </si>
   <si>
-    <t>Number</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -357,9 +354,6 @@
     <t>Been at company since 1997</t>
   </si>
   <si>
-    <t>Enjoys long walks along the beach</t>
-  </si>
-  <si>
     <t>Los Angeles, CA</t>
   </si>
   <si>
@@ -414,7 +408,10 @@
     <t>Enjoys long walks along the beach in Mexico</t>
   </si>
   <si>
-    <t>id</t>
+    <t>LeadScore</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -777,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="K3" workbookViewId="0">
+      <selection sqref="A1:P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,7 +788,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -853,90 +850,90 @@
         <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>44</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>45</v>
       </c>
-      <c r="D3" t="s">
-        <v>46</v>
-      </c>
       <c r="E3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -956,7 +953,7 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G4" t="s">
         <v>21</v>
@@ -1003,40 +1000,40 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" t="s">
         <v>113</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
+        <v>108</v>
+      </c>
+      <c r="I5" t="s">
+        <v>113</v>
+      </c>
+      <c r="J5" t="s">
+        <v>114</v>
+      </c>
+      <c r="K5" t="s">
+        <v>114</v>
+      </c>
+      <c r="L5" t="s">
+        <v>108</v>
+      </c>
+      <c r="M5" t="s">
         <v>115</v>
       </c>
-      <c r="H5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I5" t="s">
-        <v>115</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="N5" t="s">
         <v>116</v>
       </c>
-      <c r="K5" t="s">
+      <c r="O5" t="s">
         <v>116</v>
       </c>
-      <c r="L5" t="s">
-        <v>109</v>
-      </c>
-      <c r="M5" t="s">
-        <v>117</v>
-      </c>
-      <c r="N5" t="s">
-        <v>118</v>
-      </c>
-      <c r="O5" t="s">
-        <v>118</v>
-      </c>
       <c r="P5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1053,74 +1050,74 @@
         <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" t="s">
         <v>119</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>120</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>121</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>122</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>123</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>124</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>125</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>126</v>
       </c>
-      <c r="N6" t="s">
+      <c r="P6" t="s">
         <v>127</v>
-      </c>
-      <c r="O6" t="s">
-        <v>128</v>
-      </c>
-      <c r="P6" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
         <v>58</v>
       </c>
-      <c r="D8" t="s">
-        <v>59</v>
-      </c>
       <c r="E8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1137,34 +1134,34 @@
         <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F9" t="s">
         <v>22</v>
       </c>
       <c r="H9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I9" t="s">
         <v>22</v>
       </c>
       <c r="K9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L9" t="s">
         <v>22</v>
       </c>
       <c r="M9" t="s">
+        <v>62</v>
+      </c>
+      <c r="N9" t="s">
         <v>63</v>
-      </c>
-      <c r="N9" t="s">
-        <v>64</v>
       </c>
       <c r="O9" t="s">
         <v>22</v>
       </c>
       <c r="P9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1210,60 +1207,60 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -1280,40 +1277,40 @@
         <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -1330,40 +1327,40 @@
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -1380,31 +1377,31 @@
         <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N15" t="s">
         <v>12</v>
@@ -1430,348 +1427,398 @@
         <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" t="s">
-        <v>83</v>
-      </c>
-      <c r="G17" t="s">
-        <v>83</v>
-      </c>
-      <c r="H17" t="s">
-        <v>83</v>
-      </c>
-      <c r="I17" t="s">
-        <v>83</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>94</v>
+        <v>129</v>
+      </c>
+      <c r="B17">
+        <v>45</v>
+      </c>
+      <c r="C17">
+        <v>45</v>
+      </c>
+      <c r="D17">
+        <v>45</v>
+      </c>
+      <c r="E17">
+        <v>92</v>
+      </c>
+      <c r="F17">
+        <v>92</v>
+      </c>
+      <c r="G17">
+        <v>92</v>
+      </c>
+      <c r="H17">
+        <v>92</v>
+      </c>
+      <c r="I17">
+        <v>92</v>
+      </c>
+      <c r="J17">
+        <v>87</v>
+      </c>
+      <c r="K17">
+        <v>87</v>
+      </c>
+      <c r="L17">
+        <v>74</v>
+      </c>
+      <c r="M17">
+        <v>74</v>
+      </c>
+      <c r="N17">
+        <v>38</v>
+      </c>
+      <c r="O17">
+        <v>38</v>
+      </c>
+      <c r="P17">
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" t="s">
+        <v>82</v>
+      </c>
+      <c r="H18" t="s">
+        <v>82</v>
+      </c>
+      <c r="I18" t="s">
+        <v>82</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>29</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>29</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>29</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
         <v>29</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F19" t="s">
         <v>29</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G19" t="s">
         <v>29</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H19" t="s">
         <v>29</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I19" t="s">
         <v>29</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J19" t="s">
         <v>29</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K19" t="s">
         <v>29</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L19" t="s">
         <v>29</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M19" t="s">
         <v>29</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N19" t="s">
         <v>29</v>
       </c>
-      <c r="O18" t="s">
+      <c r="O19" t="s">
         <v>29</v>
       </c>
-      <c r="P18" t="s">
+      <c r="P19" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" t="s">
-        <v>30</v>
-      </c>
-      <c r="I19" t="s">
-        <v>30</v>
-      </c>
-      <c r="J19" t="s">
-        <v>30</v>
-      </c>
-      <c r="K19" t="s">
-        <v>30</v>
-      </c>
-      <c r="L19" t="s">
-        <v>30</v>
-      </c>
-      <c r="M19" t="s">
-        <v>30</v>
-      </c>
-      <c r="N19" t="s">
-        <v>30</v>
-      </c>
-      <c r="O19" t="s">
-        <v>30</v>
-      </c>
-      <c r="P19" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" t="s">
+        <v>30</v>
+      </c>
+      <c r="I20" t="s">
+        <v>30</v>
+      </c>
+      <c r="J20" t="s">
+        <v>30</v>
+      </c>
+      <c r="K20" t="s">
+        <v>30</v>
+      </c>
+      <c r="L20" t="s">
+        <v>30</v>
+      </c>
+      <c r="M20" t="s">
+        <v>30</v>
+      </c>
+      <c r="N20" t="s">
+        <v>30</v>
+      </c>
+      <c r="O20" t="s">
+        <v>30</v>
+      </c>
+      <c r="P20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>31</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>31</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>31</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" t="s">
         <v>31</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F21" t="s">
         <v>31</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" t="s">
         <v>31</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H21" t="s">
         <v>31</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I21" t="s">
         <v>31</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J21" t="s">
         <v>31</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K21" t="s">
         <v>31</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L21" t="s">
         <v>31</v>
       </c>
-      <c r="M20" t="s">
+      <c r="M21" t="s">
         <v>31</v>
       </c>
-      <c r="N20" t="s">
+      <c r="N21" t="s">
         <v>31</v>
       </c>
-      <c r="O20" t="s">
+      <c r="O21" t="s">
         <v>31</v>
       </c>
-      <c r="P20" t="s">
+      <c r="P21" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F21" t="s">
-        <v>32</v>
-      </c>
-      <c r="G21" t="s">
-        <v>32</v>
-      </c>
-      <c r="H21" t="s">
-        <v>32</v>
-      </c>
-      <c r="I21" t="s">
-        <v>32</v>
-      </c>
-      <c r="J21" t="s">
-        <v>32</v>
-      </c>
-      <c r="K21" t="s">
-        <v>32</v>
-      </c>
-      <c r="L21" t="s">
-        <v>32</v>
-      </c>
-      <c r="M21" t="s">
-        <v>32</v>
-      </c>
-      <c r="N21" t="s">
-        <v>32</v>
-      </c>
-      <c r="O21" t="s">
-        <v>32</v>
-      </c>
-      <c r="P21" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I22" t="s">
+        <v>32</v>
+      </c>
+      <c r="J22" t="s">
+        <v>32</v>
+      </c>
+      <c r="K22" t="s">
+        <v>32</v>
+      </c>
+      <c r="L22" t="s">
+        <v>32</v>
+      </c>
+      <c r="M22" t="s">
+        <v>32</v>
+      </c>
+      <c r="N22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O22" t="s">
+        <v>32</v>
+      </c>
+      <c r="P22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>33</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>33</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>33</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" t="s">
         <v>33</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F23" t="s">
         <v>33</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G23" t="s">
         <v>33</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H23" t="s">
         <v>33</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I23" t="s">
         <v>33</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J23" t="s">
         <v>33</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K23" t="s">
         <v>33</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L23" t="s">
         <v>33</v>
       </c>
-      <c r="M22" t="s">
+      <c r="M23" t="s">
         <v>33</v>
       </c>
-      <c r="N22" t="s">
+      <c r="N23" t="s">
         <v>33</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O23" t="s">
         <v>33</v>
       </c>
-      <c r="P22" t="s">
+      <c r="P23" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1"/>
-    <hyperlink ref="B17" r:id="rId2"/>
-    <hyperlink ref="C17" r:id="rId3"/>
-    <hyperlink ref="D17" r:id="rId4"/>
+    <hyperlink ref="B18" r:id="rId2"/>
+    <hyperlink ref="C18" r:id="rId3"/>
+    <hyperlink ref="D18" r:id="rId4"/>
     <hyperlink ref="C9" r:id="rId5"/>
     <hyperlink ref="D9" r:id="rId6"/>
     <hyperlink ref="C10" r:id="rId7"/>
@@ -1810,18 +1857,18 @@
     <hyperlink ref="I12" r:id="rId40"/>
     <hyperlink ref="L12" r:id="rId41"/>
     <hyperlink ref="P11" r:id="rId42"/>
-    <hyperlink ref="E17" r:id="rId43"/>
-    <hyperlink ref="F17" r:id="rId44"/>
-    <hyperlink ref="G17" r:id="rId45"/>
-    <hyperlink ref="H17" r:id="rId46"/>
-    <hyperlink ref="I17" r:id="rId47"/>
-    <hyperlink ref="N17" r:id="rId48"/>
-    <hyperlink ref="O17" r:id="rId49"/>
-    <hyperlink ref="P17" r:id="rId50"/>
-    <hyperlink ref="J17" r:id="rId51"/>
-    <hyperlink ref="K17" r:id="rId52"/>
-    <hyperlink ref="L17" r:id="rId53"/>
-    <hyperlink ref="M17" r:id="rId54"/>
+    <hyperlink ref="E18" r:id="rId43"/>
+    <hyperlink ref="F18" r:id="rId44"/>
+    <hyperlink ref="G18" r:id="rId45"/>
+    <hyperlink ref="H18" r:id="rId46"/>
+    <hyperlink ref="I18" r:id="rId47"/>
+    <hyperlink ref="N18" r:id="rId48"/>
+    <hyperlink ref="O18" r:id="rId49"/>
+    <hyperlink ref="P18" r:id="rId50"/>
+    <hyperlink ref="J18" r:id="rId51"/>
+    <hyperlink ref="K18" r:id="rId52"/>
+    <hyperlink ref="L18" r:id="rId53"/>
+    <hyperlink ref="M18" r:id="rId54"/>
     <hyperlink ref="E3" r:id="rId55"/>
     <hyperlink ref="F3" r:id="rId56"/>
     <hyperlink ref="G3" r:id="rId57"/>
@@ -1842,23 +1889,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V16"/>
+  <dimension ref="A1:W16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
         <v>35</v>
@@ -1870,10 +1917,10 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I1" t="s">
         <v>36</v>
@@ -1882,10 +1929,10 @@
         <v>37</v>
       </c>
       <c r="K1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" t="s">
         <v>52</v>
-      </c>
-      <c r="L1" t="s">
-        <v>53</v>
       </c>
       <c r="M1" t="s">
         <v>0</v>
@@ -1900,25 +1947,28 @@
         <v>13</v>
       </c>
       <c r="Q1" t="s">
+        <v>129</v>
+      </c>
+      <c r="R1" t="s">
         <v>34</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>38</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>39</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>40</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1926,7 +1976,7 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -1938,10 +1988,10 @@
         <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I2" t="s">
         <v>17</v>
@@ -1950,10 +2000,10 @@
         <v>5</v>
       </c>
       <c r="K2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" t="s">
         <v>54</v>
-      </c>
-      <c r="L2" t="s">
-        <v>55</v>
       </c>
       <c r="M2" t="s">
         <v>8</v>
@@ -1967,26 +2017,29 @@
       <c r="P2" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2">
+        <v>45</v>
+      </c>
+      <c r="R2" t="s">
         <v>16</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>29</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>30</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>31</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>32</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1994,7 +2047,7 @@
         <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -2006,10 +2059,10 @@
         <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I3" t="s">
         <v>22</v>
@@ -2018,7 +2071,7 @@
         <v>27</v>
       </c>
       <c r="K3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M3" t="s">
         <v>8</v>
@@ -2032,26 +2085,29 @@
       <c r="P3" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3">
+        <v>45</v>
+      </c>
+      <c r="R3" t="s">
         <v>16</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>29</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>30</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>31</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>32</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2059,7 +2115,7 @@
         <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -2071,10 +2127,10 @@
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I4" t="s">
         <v>23</v>
@@ -2083,7 +2139,7 @@
         <v>28</v>
       </c>
       <c r="L4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M4" t="s">
         <v>8</v>
@@ -2097,102 +2153,108 @@
       <c r="P4" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4">
+        <v>45</v>
+      </c>
+      <c r="R4" t="s">
         <v>16</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>29</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>30</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>31</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>32</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" t="s">
         <v>109</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>110</v>
       </c>
-      <c r="G5" t="s">
-        <v>111</v>
-      </c>
       <c r="H5" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="I5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M5" t="s">
+        <v>78</v>
+      </c>
+      <c r="N5" t="s">
         <v>79</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>80</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>81</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5">
+        <v>92</v>
+      </c>
+      <c r="R5" t="s">
         <v>82</v>
       </c>
-      <c r="Q5" t="s">
-        <v>83</v>
-      </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>29</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>30</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>31</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>32</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I6" t="s">
         <v>22</v>
@@ -2201,517 +2263,544 @@
         <v>27</v>
       </c>
       <c r="K6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M6" t="s">
+        <v>78</v>
+      </c>
+      <c r="N6" t="s">
         <v>79</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>80</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>81</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6">
+        <v>92</v>
+      </c>
+      <c r="R6" t="s">
         <v>82</v>
       </c>
-      <c r="Q6" t="s">
-        <v>83</v>
-      </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>29</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>30</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>31</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>32</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J7" t="s">
         <v>28</v>
       </c>
       <c r="L7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M7" t="s">
+        <v>78</v>
+      </c>
+      <c r="N7" t="s">
         <v>79</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>80</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>81</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7">
+        <v>92</v>
+      </c>
+      <c r="R7" t="s">
         <v>82</v>
       </c>
-      <c r="Q7" t="s">
-        <v>83</v>
-      </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>29</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>30</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>31</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>32</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J8" t="s">
         <v>5</v>
       </c>
       <c r="K8" t="s">
+        <v>53</v>
+      </c>
+      <c r="L8" t="s">
         <v>54</v>
       </c>
-      <c r="L8" t="s">
-        <v>55</v>
-      </c>
       <c r="M8" t="s">
+        <v>78</v>
+      </c>
+      <c r="N8" t="s">
         <v>79</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>80</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>81</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8">
+        <v>92</v>
+      </c>
+      <c r="R8" t="s">
         <v>82</v>
       </c>
-      <c r="Q8" t="s">
-        <v>83</v>
-      </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>29</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>30</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>31</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>32</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I9" t="s">
         <v>22</v>
       </c>
       <c r="K9" t="s">
+        <v>55</v>
+      </c>
+      <c r="L9" t="s">
         <v>56</v>
       </c>
-      <c r="L9" t="s">
-        <v>57</v>
-      </c>
       <c r="M9" t="s">
+        <v>78</v>
+      </c>
+      <c r="N9" t="s">
         <v>79</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>80</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>81</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9">
+        <v>92</v>
+      </c>
+      <c r="R9" t="s">
         <v>82</v>
       </c>
-      <c r="Q9" t="s">
-        <v>83</v>
-      </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>29</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>30</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>31</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>32</v>
       </c>
-      <c r="V9" t="s">
+      <c r="W9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D10" t="s">
         <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J10" t="s">
         <v>28</v>
       </c>
       <c r="M10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P10" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>95</v>
+        <v>88</v>
+      </c>
+      <c r="Q10">
+        <v>87</v>
       </c>
       <c r="R10" t="s">
+        <v>94</v>
+      </c>
+      <c r="S10" t="s">
         <v>29</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>30</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>31</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>32</v>
       </c>
-      <c r="V10" t="s">
+      <c r="W10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J11" t="s">
         <v>5</v>
       </c>
       <c r="K11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P11" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>95</v>
+        <v>88</v>
+      </c>
+      <c r="Q11">
+        <v>87</v>
       </c>
       <c r="R11" t="s">
+        <v>94</v>
+      </c>
+      <c r="S11" t="s">
         <v>29</v>
       </c>
-      <c r="S11" t="s">
+      <c r="T11" t="s">
         <v>30</v>
       </c>
-      <c r="T11" t="s">
+      <c r="U11" t="s">
         <v>31</v>
       </c>
-      <c r="U11" t="s">
+      <c r="V11" t="s">
         <v>32</v>
       </c>
-      <c r="V11" t="s">
+      <c r="W11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I12" t="s">
         <v>22</v>
       </c>
       <c r="K12" t="s">
+        <v>55</v>
+      </c>
+      <c r="L12" t="s">
         <v>56</v>
       </c>
-      <c r="L12" t="s">
-        <v>57</v>
-      </c>
       <c r="M12" t="s">
+        <v>86</v>
+      </c>
+      <c r="N12" t="s">
+        <v>85</v>
+      </c>
+      <c r="O12" t="s">
+        <v>80</v>
+      </c>
+      <c r="P12" t="s">
         <v>87</v>
       </c>
-      <c r="N12" t="s">
-        <v>86</v>
-      </c>
-      <c r="O12" t="s">
-        <v>81</v>
-      </c>
-      <c r="P12" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>96</v>
+      <c r="Q12">
+        <v>74</v>
       </c>
       <c r="R12" t="s">
+        <v>95</v>
+      </c>
+      <c r="S12" t="s">
         <v>29</v>
       </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
         <v>30</v>
       </c>
-      <c r="T12" t="s">
+      <c r="U12" t="s">
         <v>31</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="s">
         <v>32</v>
       </c>
-      <c r="V12" t="s">
+      <c r="W12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J13" t="s">
         <v>28</v>
       </c>
       <c r="M13" t="s">
+        <v>86</v>
+      </c>
+      <c r="N13" t="s">
+        <v>85</v>
+      </c>
+      <c r="O13" t="s">
+        <v>80</v>
+      </c>
+      <c r="P13" t="s">
         <v>87</v>
       </c>
-      <c r="N13" t="s">
-        <v>86</v>
-      </c>
-      <c r="O13" t="s">
-        <v>81</v>
-      </c>
-      <c r="P13" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>96</v>
+      <c r="Q13">
+        <v>74</v>
       </c>
       <c r="R13" t="s">
+        <v>95</v>
+      </c>
+      <c r="S13" t="s">
         <v>29</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>30</v>
       </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
         <v>31</v>
       </c>
-      <c r="U13" t="s">
+      <c r="V13" t="s">
         <v>32</v>
       </c>
-      <c r="V13" t="s">
+      <c r="W13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J14" t="s">
         <v>5</v>
       </c>
       <c r="M14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O14" t="s">
         <v>12</v>
       </c>
       <c r="P14" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q14">
+        <v>38</v>
+      </c>
+      <c r="R14" t="s">
         <v>93</v>
       </c>
-      <c r="Q14" t="s">
-        <v>94</v>
-      </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>29</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>30</v>
       </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
         <v>31</v>
       </c>
-      <c r="U14" t="s">
+      <c r="V14" t="s">
         <v>32</v>
       </c>
-      <c r="V14" t="s">
+      <c r="W14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D15" t="s">
         <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I15" t="s">
         <v>22</v>
@@ -2720,98 +2809,104 @@
         <v>27</v>
       </c>
       <c r="K15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O15" t="s">
         <v>12</v>
       </c>
       <c r="P15" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q15">
+        <v>38</v>
+      </c>
+      <c r="R15" t="s">
         <v>93</v>
       </c>
-      <c r="Q15" t="s">
-        <v>94</v>
-      </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>29</v>
       </c>
-      <c r="S15" t="s">
+      <c r="T15" t="s">
         <v>30</v>
       </c>
-      <c r="T15" t="s">
+      <c r="U15" t="s">
         <v>31</v>
       </c>
-      <c r="U15" t="s">
+      <c r="V15" t="s">
         <v>32</v>
       </c>
-      <c r="V15" t="s">
+      <c r="W15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D16" t="s">
         <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J16" t="s">
         <v>28</v>
       </c>
       <c r="K16" t="s">
+        <v>55</v>
+      </c>
+      <c r="L16" t="s">
         <v>56</v>
       </c>
-      <c r="L16" t="s">
-        <v>57</v>
-      </c>
       <c r="M16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O16" t="s">
         <v>12</v>
       </c>
       <c r="P16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q16">
+        <v>38</v>
+      </c>
+      <c r="R16" t="s">
         <v>93</v>
       </c>
-      <c r="Q16" t="s">
-        <v>94</v>
-      </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>29</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
         <v>30</v>
       </c>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
         <v>31</v>
       </c>
-      <c r="U16" t="s">
+      <c r="V16" t="s">
         <v>32</v>
       </c>
-      <c r="V16" t="s">
+      <c r="W16" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add nicer ph #s to data
</commit_message>
<xml_diff>
--- a/data/leads.xlsx
+++ b/data/leads.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="132">
   <si>
     <t>Company</t>
   </si>
@@ -412,6 +412,9 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>858-222-1234</t>
   </si>
 </sst>
 </file>
@@ -950,40 +953,40 @@
         <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>131</v>
       </c>
       <c r="F4" t="s">
         <v>112</v>
       </c>
       <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
         <v>21</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
+        <v>131</v>
+      </c>
+      <c r="K4" t="s">
+        <v>112</v>
+      </c>
+      <c r="L4" t="s">
         <v>7</v>
       </c>
-      <c r="I4" t="s">
+      <c r="M4" t="s">
         <v>20</v>
       </c>
-      <c r="J4" t="s">
+      <c r="N4" t="s">
         <v>21</v>
       </c>
-      <c r="K4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" t="s">
-        <v>7</v>
-      </c>
       <c r="O4" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="P4" t="s">
-        <v>21</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1468,13 +1471,13 @@
         <v>129</v>
       </c>
       <c r="B17">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="C17">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="D17">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="E17">
         <v>92</v>
@@ -2018,7 +2021,7 @@
         <v>14</v>
       </c>
       <c r="Q2">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="R2" t="s">
         <v>16</v>
@@ -2086,7 +2089,7 @@
         <v>14</v>
       </c>
       <c r="Q3">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="R3" t="s">
         <v>16</v>
@@ -2154,7 +2157,7 @@
         <v>14</v>
       </c>
       <c r="Q4">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="R4" t="s">
         <v>16</v>
@@ -2186,7 +2189,7 @@
         <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>131</v>
       </c>
       <c r="E5" t="s">
         <v>108</v>
@@ -2310,7 +2313,7 @@
         <v>98</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
         <v>113</v>
@@ -2369,7 +2372,7 @@
         <v>99</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
         <v>108</v>
@@ -2434,7 +2437,7 @@
         <v>100</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
         <v>113</v>
@@ -2496,7 +2499,7 @@
         <v>101</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>131</v>
       </c>
       <c r="E10" t="s">
         <v>114</v>
@@ -2552,7 +2555,7 @@
         <v>102</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>112</v>
       </c>
       <c r="E11" t="s">
         <v>114</v>
@@ -2614,7 +2617,7 @@
         <v>103</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
         <v>108</v>
@@ -2676,7 +2679,7 @@
         <v>104</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
         <v>115</v>
@@ -2735,7 +2738,7 @@
         <v>105</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="E14" t="s">
         <v>116</v>
@@ -2794,7 +2797,7 @@
         <v>106</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="E15" t="s">
         <v>116</v>
@@ -2856,7 +2859,7 @@
         <v>107</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>112</v>
       </c>
       <c r="E16" t="s">
         <v>116</v>

</xml_diff>